<commit_message>
Final Updated Rubric - Ibrahim
</commit_message>
<xml_diff>
--- a/management/Final Project Rubric-2.xlsx
+++ b/management/Final Project Rubric-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ibrahimhakim/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C8E656-FCF3-E943-A803-A84132735154}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C21009-9542-0643-B736-304E2032BB73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="19040" windowHeight="13600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,9 +154,6 @@
     <t>in “/management/Screenshots_Somali.pdf”: PDF screenshots as played on a PC running Linux Mint</t>
   </si>
   <si>
-    <t>Machine description (screenshot)</t>
-  </si>
-  <si>
     <t>screenshots in pdf file</t>
   </si>
   <si>
@@ -365,6 +362,9 @@
   </si>
   <si>
     <t>Line 72, specific Exception if user does not choose the following 'if else' letter options from line 61-69. Thus displaying a custom exception type</t>
+  </si>
+  <si>
+    <t>management/Ibrahim_Python_Screenshot, "ibrahim.py" is in management/ibrahim.py</t>
   </si>
 </sst>
 </file>
@@ -937,7 +937,7 @@
   <dimension ref="A1:AMK29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1013,19 +1013,19 @@
         <v>13</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -1034,19 +1034,19 @@
         <v>14</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>80</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>15</v>
@@ -1237,13 +1237,13 @@
         <v>38</v>
       </c>
       <c r="G18" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="I18" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1251,7 +1251,7 @@
         <v>26</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="13">
@@ -1261,16 +1261,16 @@
         <v>37</v>
       </c>
       <c r="F19" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="I19" s="14" t="s">
         <v>42</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>43</v>
       </c>
       <c r="J19" s="22"/>
     </row>
@@ -1279,7 +1279,7 @@
         <v>26</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="13">
@@ -1289,16 +1289,16 @@
         <v>37</v>
       </c>
       <c r="F20" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="I20" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="G20" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1306,7 +1306,7 @@
         <v>26</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="12"/>
       <c r="D21" s="13">
@@ -1316,16 +1316,16 @@
         <v>37</v>
       </c>
       <c r="F21" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="I21" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="G21" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1333,7 +1333,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="13">
@@ -1343,16 +1343,16 @@
         <v>37</v>
       </c>
       <c r="F22" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="I22" s="14" t="s">
         <v>51</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1360,7 +1360,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="13">
@@ -1370,16 +1370,16 @@
         <v>37</v>
       </c>
       <c r="F23" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="I23" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1387,7 +1387,7 @@
         <v>26</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="13">
@@ -1397,16 +1397,16 @@
         <v>37</v>
       </c>
       <c r="F24" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="I24" s="14" t="s">
         <v>57</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1414,7 +1414,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="13">
@@ -1424,16 +1424,16 @@
         <v>37</v>
       </c>
       <c r="F25" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="I25" s="14" t="s">
         <v>60</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I25" s="14" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="17" x14ac:dyDescent="0.2">
@@ -1441,14 +1441,14 @@
         <v>26</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="13">
         <v>8</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F26" s="22" t="s">
         <v>37</v>
@@ -1468,14 +1468,14 @@
         <v>26</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="13">
         <v>8</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F27" s="22" t="s">
         <v>37</v>
@@ -1496,7 +1496,7 @@
     </row>
     <row r="29" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B29" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C29" s="25">
         <f>SUM(C10:C27)</f>
@@ -1542,7 +1542,7 @@
     <row r="1" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -1563,7 +1563,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="28">
@@ -1576,7 +1576,7 @@
         <v>26</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="28">
@@ -1589,14 +1589,14 @@
         <v>26</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="28">
         <v>0.2</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1604,7 +1604,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="28">
@@ -1617,7 +1617,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="28">
@@ -1627,7 +1627,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="26">
         <f>SUM(C3:C7)</f>
@@ -1673,7 +1673,7 @@
     <row r="1" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -1694,7 +1694,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="28">
@@ -1707,7 +1707,7 @@
         <v>26</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="28">
@@ -1720,14 +1720,14 @@
         <v>26</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="28">
         <v>0.2</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1735,7 +1735,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="28">
@@ -1748,7 +1748,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="28">
@@ -1758,7 +1758,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="26">
         <f>SUM(C3:C7)</f>
@@ -1804,7 +1804,7 @@
     <row r="1" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -1825,7 +1825,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="28">
@@ -1838,7 +1838,7 @@
         <v>26</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="28">
@@ -1851,14 +1851,14 @@
         <v>26</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="28">
         <v>0.2</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1866,7 +1866,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="28">
@@ -1879,7 +1879,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="28">
@@ -1889,7 +1889,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="26">
         <f>SUM(C3:C7)</f>
@@ -1935,7 +1935,7 @@
     <row r="1" spans="1:9" ht="26.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
       <c r="B1" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31"/>
@@ -1956,7 +1956,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="28">
@@ -1969,7 +1969,7 @@
         <v>26</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="28">
@@ -1982,14 +1982,14 @@
         <v>26</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="28">
         <v>0.2</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -1997,7 +1997,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="28">
@@ -2010,7 +2010,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="28">
@@ -2020,7 +2020,7 @@
     </row>
     <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C8" s="26">
         <f>SUM(C3:C7)</f>

</xml_diff>